<commit_message>
Zeiterfassung / Funktionen angepasst
</commit_message>
<xml_diff>
--- a/Dokumente/Systemdokumentation/Funktionsbereiche & Funktionen.xlsx
+++ b/Dokumente/Systemdokumentation/Funktionsbereiche & Funktionen.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\majad\Documents\GitHub\259035_SoftEngPR\Dokumente\Systemdokumentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Cloud\Github\259035_SoftEngPR\Dokumente\Systemdokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
+    <workbookView xWindow="930" yWindow="0" windowWidth="20490" windowHeight="7530"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,18 +25,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
   <si>
     <t>Grundfunktionen</t>
-  </si>
-  <si>
-    <t>geplante Soll Zeit</t>
-  </si>
-  <si>
-    <t>Ist Zeit</t>
-  </si>
-  <si>
-    <t>Differenz</t>
   </si>
   <si>
     <t>Erstellen von Projekten</t>
@@ -155,12 +146,24 @@
   <si>
     <t>Summe</t>
   </si>
+  <si>
+    <t>geplante Soll Zeit (h)</t>
+  </si>
+  <si>
+    <t>Ist Zeit (h)</t>
+  </si>
+  <si>
+    <t>Differenz (h)</t>
+  </si>
+  <si>
+    <t>Gesamt Entwicklungszeit (h)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -182,6 +185,23 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u val="double"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -197,21 +217,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -227,7 +238,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -237,21 +248,22 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="46" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -563,31 +575,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D37"/>
+  <dimension ref="A2:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="75.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.7265625" customWidth="1"/>
-    <col min="3" max="3" width="13.26953125" customWidth="1"/>
+    <col min="1" max="1" width="67.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>2</v>
-      </c>
       <c r="D2" s="4" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -600,151 +613,159 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="8">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="8">
-        <f>B4-C4</f>
-        <v>0.33333333333333331</v>
+        <v>1</v>
+      </c>
+      <c r="B4" s="6">
+        <v>40</v>
+      </c>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6">
+        <f t="shared" ref="D4:D13" si="0">B4-C4</f>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="8">
-        <v>9.375E-2</v>
-      </c>
-      <c r="C5" s="11"/>
-      <c r="D5" s="8">
-        <f>B5-C5</f>
-        <v>9.375E-2</v>
+        <v>2</v>
+      </c>
+      <c r="B5" s="6">
+        <v>11.25</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6">
+        <f t="shared" si="0"/>
+        <v>11.25</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="8">
-        <v>0.125</v>
-      </c>
-      <c r="C6" s="11"/>
-      <c r="D6" s="8">
-        <f>B6-C6</f>
-        <v>0.125</v>
+        <v>3</v>
+      </c>
+      <c r="B6" s="6">
+        <v>15</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6">
+        <f t="shared" si="0"/>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="8">
-        <v>5.2083333333333336E-2</v>
-      </c>
-      <c r="C7" s="11"/>
-      <c r="D7" s="8">
-        <f>B7-C7</f>
-        <v>5.2083333333333336E-2</v>
+        <v>4</v>
+      </c>
+      <c r="B7" s="6">
+        <v>6.25</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6">
+        <f t="shared" si="0"/>
+        <v>6.25</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="8">
-        <v>6.25E-2</v>
-      </c>
-      <c r="C8" s="11"/>
-      <c r="D8" s="8">
-        <f>B8-C8</f>
-        <v>6.25E-2</v>
+        <v>5</v>
+      </c>
+      <c r="B8" s="6">
+        <v>7.5</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6">
+        <f t="shared" si="0"/>
+        <v>7.5</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="8">
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="8">
-        <f>B9-C9</f>
-        <v>0.16666666666666666</v>
+        <v>6</v>
+      </c>
+      <c r="B9" s="6">
+        <v>20</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6">
+        <f t="shared" si="0"/>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="8">
-        <v>5.2083333333333336E-2</v>
-      </c>
-      <c r="C10" s="11"/>
-      <c r="D10" s="8">
-        <f>B10-C10</f>
-        <v>5.2083333333333336E-2</v>
+        <v>7</v>
+      </c>
+      <c r="B10" s="6">
+        <v>6.25</v>
+      </c>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6">
+        <f t="shared" si="0"/>
+        <v>6.25</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="8">
-        <v>6.25E-2</v>
-      </c>
-      <c r="C11" s="11"/>
-      <c r="D11" s="8">
-        <f>B11-C11</f>
-        <v>6.25E-2</v>
+        <v>8</v>
+      </c>
+      <c r="B11" s="6">
+        <v>7.5</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6">
+        <f t="shared" si="0"/>
+        <v>7.5</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="8">
-        <v>5.2083333333333336E-2</v>
-      </c>
-      <c r="C12" s="11"/>
-      <c r="D12" s="8">
-        <f>B12-C12</f>
-        <v>5.2083333333333336E-2</v>
+        <v>9</v>
+      </c>
+      <c r="B12" s="6">
+        <v>6.25</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6">
+        <f t="shared" si="0"/>
+        <v>6.25</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="9">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="C13" s="12"/>
-      <c r="D13" s="9">
-        <f>B13-C13</f>
-        <v>4.1666666666666664E-2</v>
+      <c r="A13" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="6">
+        <v>5</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6">
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" s="11">
+      <c r="A14" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="8">
         <f>SUM(B4:B13)</f>
-        <v>1.0416666666666667</v>
-      </c>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11">
+        <v>125</v>
+      </c>
+      <c r="C14" s="8">
+        <f>SUM(C4:C13)</f>
+        <v>0</v>
+      </c>
+      <c r="D14" s="8">
         <f>SUM(D4:D13)</f>
-        <v>1.0416666666666667</v>
-      </c>
+        <v>125</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -752,72 +773,81 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="8">
-        <v>0.1875</v>
-      </c>
-      <c r="D17" s="8">
+        <v>12</v>
+      </c>
+      <c r="B17" s="6">
+        <v>22.5</v>
+      </c>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6">
         <f>B17-C17</f>
-        <v>0.1875</v>
+        <v>22.5</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="8">
-        <v>0.10416666666666667</v>
-      </c>
-      <c r="D18" s="8">
+        <v>13</v>
+      </c>
+      <c r="B18" s="6">
+        <v>12.5</v>
+      </c>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6">
         <f>B18-C18</f>
-        <v>0.10416666666666667</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" s="8">
-        <v>6.25E-2</v>
-      </c>
-      <c r="D19" s="8">
+        <v>14</v>
+      </c>
+      <c r="B19" s="6">
+        <v>7.5</v>
+      </c>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6">
         <f>B19-C19</f>
-        <v>6.25E-2</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" s="8">
-        <v>6.25E-2</v>
-      </c>
-      <c r="D20" s="8">
+        <v>15</v>
+      </c>
+      <c r="B20" s="6">
+        <v>7.5</v>
+      </c>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6">
         <f>B20-C20</f>
-        <v>6.25E-2</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A21" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B21" s="10">
+      <c r="A21" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="8">
         <f>SUM(B17:B20)</f>
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="C21" s="7">
-        <f t="shared" ref="C21:D21" si="0">SUM(C17:C20)</f>
+        <v>50</v>
+      </c>
+      <c r="C21" s="8">
+        <f t="shared" ref="C21" si="1">SUM(C17:C20)</f>
         <v>0</v>
       </c>
-      <c r="D21" s="10">
+      <c r="D21" s="8">
         <f>SUM(D17:D20)</f>
-        <v>0.41666666666666669</v>
-      </c>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -825,109 +855,124 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B24" s="8">
-        <v>0.20833333333333334</v>
-      </c>
-      <c r="D24" s="8">
+        <v>17</v>
+      </c>
+      <c r="B24" s="6">
+        <v>25</v>
+      </c>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6">
         <f>B24-C24</f>
-        <v>0.20833333333333334</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B25" s="8">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="D25" s="8">
+        <v>18</v>
+      </c>
+      <c r="B25" s="6">
+        <v>10</v>
+      </c>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6">
         <f>B25-C25</f>
-        <v>8.3333333333333329E-2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B26" s="8">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="D26" s="8">
+        <v>19</v>
+      </c>
+      <c r="B26" s="6">
+        <v>10</v>
+      </c>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6">
         <f>B26-C26</f>
-        <v>8.3333333333333329E-2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B27" s="8">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="D27" s="8">
+        <v>20</v>
+      </c>
+      <c r="B27" s="6">
+        <v>10</v>
+      </c>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6">
         <f>B27-C27</f>
-        <v>8.3333333333333329E-2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A28" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B28" s="10">
+      <c r="A28" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" s="8">
         <f>SUM(B24:B27)</f>
-        <v>0.45833333333333331</v>
-      </c>
-      <c r="C28" s="7">
-        <f t="shared" ref="C28:D28" si="1">SUM(C24:C27)</f>
+        <v>55</v>
+      </c>
+      <c r="C28" s="8">
+        <f t="shared" ref="C28" si="2">SUM(C24:C27)</f>
         <v>0</v>
       </c>
-      <c r="D28" s="10">
+      <c r="D28" s="8">
         <f>SUM(D24:D27)</f>
-        <v>0.45833333333333331</v>
-      </c>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
+        <v>21</v>
+      </c>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B31" s="8">
-        <v>0.22916666666666666</v>
-      </c>
-      <c r="D31" s="8">
+        <v>22</v>
+      </c>
+      <c r="B31" s="6">
+        <v>27.5</v>
+      </c>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6">
         <f>B31-C31</f>
-        <v>0.22916666666666666</v>
+        <v>27.5</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A32" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B32" s="10">
+      <c r="A32" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B32" s="8">
         <f>SUM(B31)</f>
-        <v>0.22916666666666666</v>
-      </c>
-      <c r="C32" s="7">
-        <f t="shared" ref="C32:D32" si="2">SUM(C31)</f>
+        <v>27.5</v>
+      </c>
+      <c r="C32" s="8">
+        <f t="shared" ref="C32" si="3">SUM(C31)</f>
         <v>0</v>
       </c>
-      <c r="D32" s="10">
+      <c r="D32" s="8">
         <f>SUM(D31)</f>
-        <v>0.22916666666666666</v>
-      </c>
+        <v>27.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -935,43 +980,56 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>27</v>
-      </c>
-      <c r="B35" s="8">
-        <v>0.125</v>
-      </c>
-      <c r="D35" s="8">
+        <v>24</v>
+      </c>
+      <c r="B35" s="6">
+        <v>15</v>
+      </c>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6">
         <f>B35-C35</f>
-        <v>0.125</v>
+        <v>15</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>28</v>
-      </c>
-      <c r="B36" s="8">
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="D36" s="8">
+        <v>25</v>
+      </c>
+      <c r="B36" s="6">
+        <v>20</v>
+      </c>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6">
         <f>B36-C36</f>
-        <v>0.16666666666666666</v>
+        <v>20</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A37" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B37" s="10">
+      <c r="A37" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B37" s="8">
         <f>SUM(B35:B36)</f>
-        <v>0.29166666666666663</v>
-      </c>
-      <c r="C37" s="7">
-        <f t="shared" ref="C37:D37" si="3">SUM(C35:C36)</f>
+        <v>35</v>
+      </c>
+      <c r="C37" s="8">
+        <f t="shared" ref="C37" si="4">SUM(C35:C36)</f>
         <v>0</v>
       </c>
-      <c r="D37" s="10">
+      <c r="D37" s="8">
         <f>SUM(D35:D36)</f>
-        <v>0.29166666666666663</v>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A40" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B40" s="11"/>
+      <c r="C40" s="11"/>
+      <c r="D40" s="10">
+        <f>D37+D32+D21+D14+D28</f>
+        <v>292.5</v>
       </c>
     </row>
   </sheetData>
@@ -986,7 +1044,7 @@
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>